<commit_message>
Update Overlay.java, board.jsp main.js, overlay.jsp, common.css and Worker Cost.xlsx
Preparing to create input elements with javascript to reuse board.jsp markup in overlay.jsp markup
</commit_message>
<xml_diff>
--- a/Design/Worker Cost.xlsx
+++ b/Design/Worker Cost.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roody\Documents\GitHub\Beggar-Office-Jsp\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F397F310-CF68-4249-8731-B709FEAE52E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB34B17-67CC-4259-9F16-173ECCD314F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{CFA388DC-BCBE-4ADA-844D-75964697FDAF}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -619,7 +619,7 @@
         <v>500000</v>
       </c>
       <c r="C7" s="3">
-        <v>1500000</v>
+        <v>950000</v>
       </c>
       <c r="D7" s="3">
         <v>3100000</v>

</xml_diff>